<commit_message>
Solved the issue with extended study and added a graph
I'm writing the SLR and I discovered there was a problem with an extended work which was deleted (correctly); we must remember that for this reason I've added an exclusion criteria, and that this choice should be correctly propagated.
Furthermore, I've created a nice graph in the appraisal excel.
</commit_message>
<xml_diff>
--- a/6_Quality Appraisal/Quality_Appraisal.xlsx
+++ b/6_Quality Appraisal/Quality_Appraisal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29101"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://communitystudentiunina.sharepoint.com/sites/PRINMEDITATE/Shared Documents/SLR/RegressionTestingOptimizationSLR/6_Quality Appraisal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoniotrovato/Documents/GitHub/RegressionTestingOptimizationSLR/6_Quality Appraisal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2666" documentId="13_ncr:1_{60034CB3-C5CB-EC4D-8E1F-7CB1A479B67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AEDCDD0-9B3C-4724-8022-2A850E641812}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBA6C62-F01F-6A40-949A-384EEDFE9D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="620" windowWidth="28800" windowHeight="15580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,10 +43,10 @@
   <commentList>
     <comment ref="AX125" authorId="0" shapeId="0" xr:uid="{ACAF5DB7-39A9-DA4F-81D5-ACC0A1571768}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    da controllare</t>
+        <t>[Commento in thread]
+La versione di Excel in uso consente di leggere questo commento in thread, ma tutte le modifiche a esso apportate verranno rimosse se il file viene aperto in una versione più recente di Excel. Ulteriori informazioni: https://go.microsoft.com/fwlink/?linkid=870924
+Commento:
+da controllare</t>
       </text>
     </comment>
   </commentList>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1781" uniqueCount="1330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1790" uniqueCount="1336">
   <si>
     <t>ID</t>
   </si>
@@ -4100,12 +4100,30 @@
   <si>
     <t>Test case prioritization assigns the execution priorities of the test cases in a given test suite. Many existing test case prioritization techniques assume the full-fledged availability of code coverage data, fault history, or test specification, which are seldom well-maintained in real-world software development projects. This paper proposes a novel family of input-based local-beam-search adaptive-randomized techniques. They make adaptive tree-based randomized explorations with a randomized candidate test set strategy to even out the search space explorations among the branches of the exploration trees constructed by the test inputs in the test suite. We report a validation experiment on a suite of four medium-size benchmarks. The results show that our techniques achieve either higher APFD values than or the same mean APFD values as the existing code-coverage-based greedy or search-based prioritization techniques, including Genetic, Greedy and ART, in both our controlled experiment and case study. Our techniques are also significantly more efficient than the Genetic and Greedy, but are less efficient than ART.</t>
   </si>
+  <si>
+    <t>AO</t>
+  </si>
+  <si>
+    <t>AN=1.0</t>
+  </si>
+  <si>
+    <t>AN=0.8</t>
+  </si>
+  <si>
+    <t>AN=0.5</t>
+  </si>
+  <si>
+    <t>AN=0.4</t>
+  </si>
+  <si>
+    <t>AN=0.2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4227,7 +4245,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4283,12 +4301,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -4305,6 +4317,1368 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$BI$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AN=1.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$BH$3:$BH$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>PS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SLR</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$BI$3:$BI$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-59E7-7544-B36B-120D29F13818}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$BJ$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AN=0.8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$BH$3:$BH$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>PS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SLR</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$BJ$3:$BJ$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-59E7-7544-B36B-120D29F13818}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$BK$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AN=0.5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$BH$3:$BH$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>PS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SLR</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$BK$3:$BK$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-59E7-7544-B36B-120D29F13818}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$BL$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AN=0.4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$BH$3:$BH$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>PS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SLR</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$BL$3:$BL$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-59E7-7544-B36B-120D29F13818}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$BM$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AN=0.2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$BH$3:$BH$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>PS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SLR</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$BM$3:$BM$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-59E7-7544-B36B-120D29F13818}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1471775615"/>
+        <c:axId val="1471788159"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1471775615"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1471788159"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1471788159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1471775615"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>60</xdr:col>
+      <xdr:colOff>481543</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>289983</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>312210</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3033183</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD88AA6F-6303-734C-2C1F-614D5A854C5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4608,35 +5982,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BI203"/>
+  <dimension ref="A1:BM203"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="AN1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BE3" sqref="BE3"/>
+      <pane xSplit="3" topLeftCell="BH1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
+      <selection pane="topRight" activeCell="BL4" sqref="BL4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="112.28515625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="76.42578125" style="7" customWidth="1"/>
-    <col min="6" max="9" width="8.85546875" style="13"/>
+    <col min="1" max="1" width="23.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="112.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="76.5" style="7" customWidth="1"/>
+    <col min="6" max="9" width="8.83203125" style="13"/>
     <col min="10" max="10" width="125" style="7" customWidth="1"/>
-    <col min="11" max="11" width="79.28515625" style="7" customWidth="1"/>
-    <col min="12" max="12" width="37.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="38" width="8.85546875" style="5"/>
-    <col min="39" max="39" width="93.140625" style="7" customWidth="1"/>
-    <col min="40" max="56" width="8.85546875" style="13"/>
-    <col min="57" max="57" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="58" max="16384" width="8.85546875" style="5"/>
+    <col min="11" max="11" width="79.33203125" style="7" customWidth="1"/>
+    <col min="12" max="12" width="37.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="38" width="8.83203125" style="5"/>
+    <col min="39" max="39" width="93.1640625" style="7" customWidth="1"/>
+    <col min="40" max="56" width="8.83203125" style="13"/>
+    <col min="57" max="57" width="9.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="58" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="17.100000000000001" thickBot="1">
+    <row r="1" spans="1:65" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4809,7 +6183,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:59" ht="50.25" customHeight="1">
+    <row r="2" spans="1:65" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>57</v>
       </c>
@@ -4893,13 +6267,31 @@
         <f>AVERAGE(BB2,BC2)</f>
         <v>0.18</v>
       </c>
-      <c r="BE2" s="19">
+      <c r="BE2" s="13">
         <f>AVERAGE(AO2,BD2)</f>
         <v>0.29000000000000004</v>
       </c>
-      <c r="BF2" s="20"/>
+      <c r="BF2" s="7"/>
+      <c r="BH2" s="5" t="s">
+        <v>1330</v>
+      </c>
+      <c r="BI2" s="5" t="s">
+        <v>1331</v>
+      </c>
+      <c r="BJ2" s="5" t="s">
+        <v>1332</v>
+      </c>
+      <c r="BK2" s="5" t="s">
+        <v>1333</v>
+      </c>
+      <c r="BL2" s="5" t="s">
+        <v>1334</v>
+      </c>
+      <c r="BM2" s="5" t="s">
+        <v>1335</v>
+      </c>
     </row>
-    <row r="3" spans="1:59" ht="255.95">
+    <row r="3" spans="1:65" ht="257" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>9022761</v>
       </c>
@@ -4973,20 +6365,42 @@
         <f t="shared" ref="BC3:BC26" si="1">AVERAGE(AQ3,AS3,AU3,AW3,AY3,BA3)</f>
         <v>0.63333333333333341</v>
       </c>
-      <c r="BD3" s="13">
-        <f t="shared" ref="BD3:BD26" si="2">AVERAGE(BB3,BC3)</f>
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="BE3" s="19">
-        <f t="shared" ref="BE3:BE26" si="3">AVERAGE(AO3,BD3)</f>
-        <v>0.54166666666666674</v>
+      <c r="BD3" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="BE3" s="13">
+        <f>AVERAGE(AO3,BD3)</f>
+        <v>0.5</v>
       </c>
       <c r="BF3" s="8"/>
       <c r="BG3" s="5" t="s">
         <v>79</v>
       </c>
+      <c r="BH3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="BI3" s="5">
+        <f>COUNTIFS($AO$2:$AO$1000,"1,0",$AN$2:$AN$1000,"PS", $BE$2:$BE$1000,"&gt;=0,6")</f>
+        <v>60</v>
+      </c>
+      <c r="BJ3" s="5">
+        <f>COUNTIFS($AO$2:$AO$1000,"0,8",$AN$2:$AN$1000,"PS", $BE$2:$BE$1000,"&gt;=0,6")</f>
+        <v>24</v>
+      </c>
+      <c r="BK3" s="5">
+        <f>COUNTIFS($AO$2:$AO$1000,"0,5",$AN$2:$AN$1000,"PS", $BE$2:$BE$1000,"&gt;=0,6")</f>
+        <v>17</v>
+      </c>
+      <c r="BL3" s="5">
+        <f>COUNTIFS($AO$2:$AO$1000,"0,4",$AN$2:$AN$1000,"PS", $BE$2:$BE$1000,"&gt;=0,6")</f>
+        <v>9</v>
+      </c>
+      <c r="BM3" s="5">
+        <f>COUNTIFS($AO$2:$AO$1000,"0,2",$AN$2:$AN$1000,"PS", $BE$2:$BE$1000,"&gt;=0,6")</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:59" ht="144">
+    <row r="4" spans="1:65" ht="145" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>7561371</v>
       </c>
@@ -5058,19 +6472,42 @@
         <v>0.63333333333333341</v>
       </c>
       <c r="BD4" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="BD3:BD26" si="2">AVERAGE(BB4,BC4)</f>
         <v>0.63333333333333341</v>
       </c>
       <c r="BE4" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="BE4:BE26" si="3">AVERAGE(AO4,BD4)</f>
         <v>0.51666666666666672</v>
       </c>
       <c r="BF4" s="10"/>
       <c r="BG4" s="5" t="s">
         <v>88</v>
       </c>
+      <c r="BH4" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="BI4" s="5">
+        <f>COUNTIFS($AO$2:$AO$1000,"1,0",$AN$2:$AN$1000,"SLR", $BE$2:$BE$1000,"&gt;=0,6")</f>
+        <v>4</v>
+      </c>
+      <c r="BJ4" s="5">
+        <f>COUNTIFS($AO$2:$AO$1000,"0,8",$AN$2:$AN$1000,"SLR", $BE$2:$BE$1000,"&gt;=0,6")</f>
+        <v>2</v>
+      </c>
+      <c r="BK4" s="5">
+        <f>COUNTIFS($AO$2:$AO$1000,"0,5",$AN$2:$AN$1000,"SLR", $BE$2:$BE$1000,"&gt;=0,6")</f>
+        <v>1</v>
+      </c>
+      <c r="BL4" s="5">
+        <f>COUNTIFS($AO$2:$AO$1000,"0,4",$AN$2:$AN$1000,"SLR", $BE$2:$BE$1000,"&gt;=0,6")</f>
+        <v>0</v>
+      </c>
+      <c r="BM4" s="5">
+        <f>COUNTIFS($AO$2:$AO$1000,"0,2",$AN$2:$AN$1000,"SLR", $BE$2:$BE$1000,"&gt;=0,6")</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:59" ht="224.1">
+    <row r="5" spans="1:65" ht="225" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>6884931</v>
       </c>
@@ -5153,8 +6590,31 @@
       <c r="BG5" s="5" t="s">
         <v>98</v>
       </c>
+      <c r="BH5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="BI5" s="5">
+        <f>COUNTIFS($AO$2:$AO$1000,"1,0",$AN$2:$AN$1000,"SR", $BE$2:$BE$1000,"&gt;=0,6")</f>
+        <v>5</v>
+      </c>
+      <c r="BJ5" s="5">
+        <f>COUNTIFS($AO$2:$AO$1000,"0,8",$AN$2:$AN$1000,"SR", $BE$2:$BE$1000,"&gt;=0,6")</f>
+        <v>2</v>
+      </c>
+      <c r="BK5" s="5">
+        <f>COUNTIFS($AO$2:$AO$1000,"0,5",$AN$2:$AN$1000,"SR", $BE$2:$BE$1000,"&gt;=0,6")</f>
+        <v>1</v>
+      </c>
+      <c r="BL5" s="5">
+        <f>COUNTIFS($AO$2:$AO$1000,"0,4",$AN$2:$AN$1000,"SR", $BE$2:$BE$1000,"&gt;=0,6")</f>
+        <v>0</v>
+      </c>
+      <c r="BM5" s="5">
+        <f>COUNTIFS($AO$2:$AO$1000,"0,2",$AN$2:$AN$1000,"SR", $BE$2:$BE$1000,"&gt;=0,6")</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:59" ht="192">
+    <row r="6" spans="1:65" ht="193" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>10048797</v>
       </c>
@@ -5250,7 +6710,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:59" ht="128.1">
+    <row r="7" spans="1:65" ht="128" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>8377903</v>
       </c>
@@ -5336,7 +6796,7 @@
         <v>0.76666666666666672</v>
       </c>
     </row>
-    <row r="8" spans="1:59" ht="192">
+    <row r="8" spans="1:65" ht="192" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>7045344</v>
       </c>
@@ -5428,7 +6888,7 @@
         <v>0.36499999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:59" ht="192">
+    <row r="9" spans="1:65" ht="192" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>9198020</v>
       </c>
@@ -5508,7 +6968,7 @@
         <v>0.53333333333333333</v>
       </c>
     </row>
-    <row r="10" spans="1:59" ht="128.1">
+    <row r="10" spans="1:65" ht="128" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>8776936</v>
       </c>
@@ -5588,7 +7048,7 @@
         <v>0.51666666666666672</v>
       </c>
     </row>
-    <row r="11" spans="1:59" ht="192">
+    <row r="11" spans="1:65" ht="192" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>10197719</v>
       </c>
@@ -5687,7 +7147,7 @@
         <v>0.71666666666666656</v>
       </c>
     </row>
-    <row r="12" spans="1:59" ht="207.95">
+    <row r="12" spans="1:65" ht="208" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>8261011</v>
       </c>
@@ -5767,7 +7227,7 @@
         <v>0.53333333333333333</v>
       </c>
     </row>
-    <row r="13" spans="1:59" ht="176.1">
+    <row r="13" spans="1:65" ht="176" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>9160217</v>
       </c>
@@ -5861,7 +7321,7 @@
         <v>0.41416666666666668</v>
       </c>
     </row>
-    <row r="14" spans="1:59" ht="176.1">
+    <row r="14" spans="1:65" ht="176" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>8229925</v>
       </c>
@@ -5941,7 +7401,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:59" ht="144">
+    <row r="15" spans="1:65" ht="144" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>7207103</v>
       </c>
@@ -6021,7 +7481,7 @@
         <v>0.58333333333333326</v>
       </c>
     </row>
-    <row r="16" spans="1:59" ht="96">
+    <row r="16" spans="1:65" ht="96" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>7515934</v>
       </c>
@@ -6101,7 +7561,7 @@
         <v>0.60833333333333328</v>
       </c>
     </row>
-    <row r="17" spans="1:60" ht="111.95">
+    <row r="17" spans="1:60" ht="112" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>6888744</v>
       </c>
@@ -6181,7 +7641,7 @@
         <v>0.6333333333333333</v>
       </c>
     </row>
-    <row r="18" spans="1:60" ht="144">
+    <row r="18" spans="1:60" ht="144" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>7019794</v>
       </c>
@@ -6261,7 +7721,7 @@
         <v>0.51666666666666661</v>
       </c>
     </row>
-    <row r="19" spans="1:60" ht="159.94999999999999">
+    <row r="19" spans="1:60" ht="160" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>7155012</v>
       </c>
@@ -6341,7 +7801,7 @@
         <v>0.53333333333333333</v>
       </c>
     </row>
-    <row r="20" spans="1:60" ht="159.94999999999999">
+    <row r="20" spans="1:60" ht="160" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>7380585</v>
       </c>
@@ -6433,7 +7893,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="21" spans="1:60" ht="128.1">
+    <row r="21" spans="1:60" ht="128" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>6949377</v>
       </c>
@@ -6513,7 +7973,7 @@
         <v>0.53333333333333333</v>
       </c>
     </row>
-    <row r="22" spans="1:60" ht="128.1">
+    <row r="22" spans="1:60" ht="128" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>7975319</v>
       </c>
@@ -6597,7 +8057,7 @@
         <v>0.48749999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:60" ht="144">
+    <row r="23" spans="1:60" ht="144" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>7809434</v>
       </c>
@@ -6677,7 +8137,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="24" spans="1:60" ht="128.1">
+    <row r="24" spans="1:60" ht="128" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>7475187</v>
       </c>
@@ -6757,7 +8217,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="25" spans="1:60" ht="176.1">
+    <row r="25" spans="1:60" ht="176" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>7148505</v>
       </c>
@@ -6837,7 +8297,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="26" spans="1:60" ht="192">
+    <row r="26" spans="1:60" ht="192" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>6571611</v>
       </c>
@@ -6917,7 +8377,7 @@
         <v>0.6333333333333333</v>
       </c>
     </row>
-    <row r="27" spans="1:60" ht="192">
+    <row r="27" spans="1:60" ht="192" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>10301343</v>
       </c>
@@ -6997,7 +8457,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="28" spans="1:60" ht="207.95">
+    <row r="28" spans="1:60" ht="208" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>8991616</v>
       </c>
@@ -7080,7 +8540,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="29" spans="1:60" ht="240">
+    <row r="29" spans="1:60" ht="240" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>9440156</v>
       </c>
@@ -7160,7 +8620,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="30" spans="1:60" ht="176.1">
+    <row r="30" spans="1:60" ht="176" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>7557497</v>
       </c>
@@ -7240,7 +8700,7 @@
         <v>0.56666666666666665</v>
       </c>
     </row>
-    <row r="31" spans="1:60" ht="288">
+    <row r="31" spans="1:60" ht="288" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>8281742</v>
       </c>
@@ -7323,7 +8783,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="32" spans="1:60" ht="192">
+    <row r="32" spans="1:60" ht="192" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>8117002</v>
       </c>
@@ -7403,7 +8863,7 @@
         <v>0.58333333333333326</v>
       </c>
     </row>
-    <row r="33" spans="1:57" ht="176.1">
+    <row r="33" spans="1:57" ht="176" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>10499739</v>
       </c>
@@ -7483,7 +8943,7 @@
         <v>0.41666666666666663</v>
       </c>
     </row>
-    <row r="34" spans="1:57" ht="176.1">
+    <row r="34" spans="1:57" ht="176" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>10199547</v>
       </c>
@@ -7563,7 +9023,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:57" ht="207.95">
+    <row r="35" spans="1:57" ht="208" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>7273631</v>
       </c>
@@ -7649,7 +9109,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="1:57" ht="111.95">
+    <row r="36" spans="1:57" ht="112" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>7885851</v>
       </c>
@@ -7729,7 +9189,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="37" spans="1:57" ht="272.10000000000002">
+    <row r="37" spans="1:57" ht="272" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>10507913</v>
       </c>
@@ -7809,7 +9269,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="38" spans="1:57" ht="176.1">
+    <row r="38" spans="1:57" ht="176" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>8305939</v>
       </c>
@@ -7889,7 +9349,7 @@
         <v>0.68333333333333335</v>
       </c>
     </row>
-    <row r="39" spans="1:57" ht="207.95">
+    <row r="39" spans="1:57" ht="208" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>9440161</v>
       </c>
@@ -7969,7 +9429,7 @@
         <v>0.53333333333333333</v>
       </c>
     </row>
-    <row r="40" spans="1:57" ht="207.95">
+    <row r="40" spans="1:57" ht="208" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>9796413</v>
       </c>
@@ -8049,7 +9509,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="41" spans="1:57" ht="192">
+    <row r="41" spans="1:57" ht="192" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>6844270</v>
       </c>
@@ -8129,7 +9589,7 @@
         <v>0.39166666666666666</v>
       </c>
     </row>
-    <row r="42" spans="1:57" ht="159.94999999999999">
+    <row r="42" spans="1:57" ht="160" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>7375627</v>
       </c>
@@ -8209,7 +9669,7 @@
         <v>0.58333333333333326</v>
       </c>
     </row>
-    <row r="43" spans="1:57" ht="159.94999999999999">
+    <row r="43" spans="1:57" ht="160" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>8452804</v>
       </c>
@@ -8286,7 +9746,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="44" spans="1:57" ht="159.94999999999999">
+    <row r="44" spans="1:57" ht="160" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>10932075</v>
       </c>
@@ -8366,7 +9826,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="45" spans="1:57" ht="207.95">
+    <row r="45" spans="1:57" ht="208" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>7273420</v>
       </c>
@@ -8452,7 +9912,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="46" spans="1:57" ht="240">
+    <row r="46" spans="1:57" ht="240" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>10298744</v>
       </c>
@@ -8535,7 +9995,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="47" spans="1:57" ht="144">
+    <row r="47" spans="1:57" ht="144" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>9787970</v>
       </c>
@@ -8618,7 +10078,7 @@
         <v>0.6333333333333333</v>
       </c>
     </row>
-    <row r="48" spans="1:57" ht="159.94999999999999">
+    <row r="48" spans="1:57" ht="160" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>8855691</v>
       </c>
@@ -8698,7 +10158,7 @@
         <v>0.6333333333333333</v>
       </c>
     </row>
-    <row r="49" spans="1:57" ht="224.1">
+    <row r="49" spans="1:57" ht="224" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>8029584</v>
       </c>
@@ -8784,7 +10244,7 @@
         <v>0.73333333333333339</v>
       </c>
     </row>
-    <row r="50" spans="1:57" ht="207.95">
+    <row r="50" spans="1:57" ht="208" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>7838169</v>
       </c>
@@ -8864,7 +10324,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="51" spans="1:57" ht="159.94999999999999">
+    <row r="51" spans="1:57" ht="160" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>6569743</v>
       </c>
@@ -8947,7 +10407,7 @@
         <v>0.76666666666666661</v>
       </c>
     </row>
-    <row r="52" spans="1:57" ht="159.94999999999999">
+    <row r="52" spans="1:57" ht="160" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>7783254</v>
       </c>
@@ -9027,7 +10487,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="53" spans="1:57" ht="159.94999999999999">
+    <row r="53" spans="1:57" ht="160" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>8854718</v>
       </c>
@@ -9107,7 +10567,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="54" spans="1:57" ht="159.94999999999999">
+    <row r="54" spans="1:57" ht="160" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>8536351</v>
       </c>
@@ -9184,7 +10644,7 @@
         <v>0.58333333333333326</v>
       </c>
     </row>
-    <row r="55" spans="1:57" ht="159.94999999999999">
+    <row r="55" spans="1:57" ht="160" x14ac:dyDescent="0.2">
       <c r="A55" s="6">
         <v>7272924</v>
       </c>
@@ -9264,7 +10724,7 @@
         <v>0.6333333333333333</v>
       </c>
     </row>
-    <row r="56" spans="1:57" ht="240">
+    <row r="56" spans="1:57" ht="240" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
         <v>9741963</v>
       </c>
@@ -9344,7 +10804,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="57" spans="1:57" ht="176.1">
+    <row r="57" spans="1:57" ht="176" x14ac:dyDescent="0.2">
       <c r="A57" s="6">
         <v>10675922</v>
       </c>
@@ -9427,7 +10887,7 @@
         <v>0.3666666666666667</v>
       </c>
     </row>
-    <row r="58" spans="1:57" ht="111.95">
+    <row r="58" spans="1:57" ht="112" x14ac:dyDescent="0.2">
       <c r="A58" s="6">
         <v>10229439</v>
       </c>
@@ -9510,7 +10970,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="59" spans="1:57" ht="159.94999999999999">
+    <row r="59" spans="1:57" ht="160" x14ac:dyDescent="0.2">
       <c r="A59" s="6">
         <v>8625203</v>
       </c>
@@ -9590,7 +11050,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="60" spans="1:57" ht="128.1">
+    <row r="60" spans="1:57" ht="128" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
         <v>6649891</v>
       </c>
@@ -9673,7 +11133,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="61" spans="1:57" ht="128.1">
+    <row r="61" spans="1:57" ht="128" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
         <v>10911525</v>
       </c>
@@ -9753,7 +11213,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="62" spans="1:57" ht="159.94999999999999">
+    <row r="62" spans="1:57" ht="160" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
         <v>10196878</v>
       </c>
@@ -9836,7 +11296,7 @@
         <v>0.6166666666666667</v>
       </c>
     </row>
-    <row r="63" spans="1:57" ht="240">
+    <row r="63" spans="1:57" ht="240" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
         <v>10366665</v>
       </c>
@@ -9919,7 +11379,7 @@
         <v>0.58333333333333326</v>
       </c>
     </row>
-    <row r="64" spans="1:57" ht="192">
+    <row r="64" spans="1:57" ht="192" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
         <v>7589817</v>
       </c>
@@ -9999,7 +11459,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="65" spans="1:57" ht="192">
+    <row r="65" spans="1:57" ht="192" x14ac:dyDescent="0.2">
       <c r="A65" s="6">
         <v>7381799</v>
       </c>
@@ -10079,7 +11539,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="66" spans="1:57" ht="207.95">
+    <row r="66" spans="1:57" ht="208" x14ac:dyDescent="0.2">
       <c r="A66" s="6">
         <v>9103716</v>
       </c>
@@ -10159,7 +11619,7 @@
         <v>0.58333333333333326</v>
       </c>
     </row>
-    <row r="67" spans="1:57" ht="240">
+    <row r="67" spans="1:57" ht="240" x14ac:dyDescent="0.2">
       <c r="A67" s="6">
         <v>10621714</v>
       </c>
@@ -10239,7 +11699,7 @@
         <v>0.76666666666666661</v>
       </c>
     </row>
-    <row r="68" spans="1:57" ht="96">
+    <row r="68" spans="1:57" ht="96" x14ac:dyDescent="0.2">
       <c r="A68" s="6">
         <v>10216597</v>
       </c>
@@ -10322,7 +11782,7 @@
         <v>0.3666666666666667</v>
       </c>
     </row>
-    <row r="69" spans="1:57" ht="192">
+    <row r="69" spans="1:57" ht="192" x14ac:dyDescent="0.2">
       <c r="A69" s="6">
         <v>7943143</v>
       </c>
@@ -10402,7 +11862,7 @@
         <v>0.53333333333333333</v>
       </c>
     </row>
-    <row r="70" spans="1:57" ht="176.1">
+    <row r="70" spans="1:57" ht="176" x14ac:dyDescent="0.2">
       <c r="A70" s="6">
         <v>9142966</v>
       </c>
@@ -10482,7 +11942,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="71" spans="1:57" ht="224.1">
+    <row r="71" spans="1:57" ht="224" x14ac:dyDescent="0.2">
       <c r="A71" s="6">
         <v>8530033</v>
       </c>
@@ -10565,7 +12025,7 @@
         <v>0.83333333333333326</v>
       </c>
     </row>
-    <row r="72" spans="1:57" ht="176.1">
+    <row r="72" spans="1:57" ht="176" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
         <v>10298714</v>
       </c>
@@ -10648,7 +12108,7 @@
         <v>0.51666666666666661</v>
       </c>
     </row>
-    <row r="73" spans="1:57" ht="144">
+    <row r="73" spans="1:57" ht="144" x14ac:dyDescent="0.2">
       <c r="A73" s="6">
         <v>8300829</v>
       </c>
@@ -10728,7 +12188,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="74" spans="1:57" ht="207.95">
+    <row r="74" spans="1:57" ht="208" x14ac:dyDescent="0.2">
       <c r="A74" s="6">
         <v>7819324</v>
       </c>
@@ -10811,7 +12271,7 @@
         <v>0.51666666666666672</v>
       </c>
     </row>
-    <row r="75" spans="1:57" ht="240">
+    <row r="75" spans="1:57" ht="240" x14ac:dyDescent="0.2">
       <c r="A75" s="6">
         <v>10062444</v>
       </c>
@@ -10894,7 +12354,7 @@
         <v>0.51666666666666661</v>
       </c>
     </row>
-    <row r="76" spans="1:57" ht="255.95">
+    <row r="76" spans="1:57" ht="256" x14ac:dyDescent="0.2">
       <c r="A76" s="6">
         <v>9825820</v>
       </c>
@@ -10977,7 +12437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:57" ht="176.1">
+    <row r="77" spans="1:57" ht="176" x14ac:dyDescent="0.2">
       <c r="A77" s="6">
         <v>7272927</v>
       </c>
@@ -11057,7 +12517,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="78" spans="1:57" ht="128.1">
+    <row r="78" spans="1:57" ht="128" x14ac:dyDescent="0.2">
       <c r="A78" s="6">
         <v>8539203</v>
       </c>
@@ -11137,7 +12597,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="79" spans="1:57" ht="192">
+    <row r="79" spans="1:57" ht="192" x14ac:dyDescent="0.2">
       <c r="A79" s="6">
         <v>6928903</v>
       </c>
@@ -11217,7 +12677,7 @@
         <v>0.71666666666666667</v>
       </c>
     </row>
-    <row r="80" spans="1:57" ht="159.94999999999999">
+    <row r="80" spans="1:57" ht="160" x14ac:dyDescent="0.2">
       <c r="A80" s="6">
         <v>6595798</v>
       </c>
@@ -11297,7 +12757,7 @@
         <v>0.53333333333333333</v>
       </c>
     </row>
-    <row r="81" spans="1:57" ht="144">
+    <row r="81" spans="1:57" ht="144" x14ac:dyDescent="0.2">
       <c r="A81" s="6">
         <v>7091286</v>
       </c>
@@ -11383,7 +12843,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="82" spans="1:57" ht="192">
+    <row r="82" spans="1:57" ht="192" x14ac:dyDescent="0.2">
       <c r="A82" s="6">
         <v>10336260</v>
       </c>
@@ -11466,7 +12926,7 @@
         <v>0.76666666666666661</v>
       </c>
     </row>
-    <row r="83" spans="1:57" ht="192">
+    <row r="83" spans="1:57" ht="192" x14ac:dyDescent="0.2">
       <c r="A83" s="6">
         <v>10304799</v>
       </c>
@@ -11546,7 +13006,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="84" spans="1:57" ht="224.1">
+    <row r="84" spans="1:57" ht="224" x14ac:dyDescent="0.2">
       <c r="A84" s="6">
         <v>10011478</v>
       </c>
@@ -11626,7 +13086,7 @@
         <v>0.71666666666666667</v>
       </c>
     </row>
-    <row r="85" spans="1:57" ht="272.10000000000002">
+    <row r="85" spans="1:57" ht="272" x14ac:dyDescent="0.2">
       <c r="A85" s="6">
         <v>9260075</v>
       </c>
@@ -11706,7 +13166,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="86" spans="1:57" ht="207.95">
+    <row r="86" spans="1:57" ht="208" x14ac:dyDescent="0.2">
       <c r="A86" s="6">
         <v>8914670</v>
       </c>
@@ -11789,7 +13249,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="87" spans="1:57" ht="224.1">
+    <row r="87" spans="1:57" ht="224" x14ac:dyDescent="0.2">
       <c r="A87" s="6">
         <v>10877022</v>
       </c>
@@ -11872,7 +13332,7 @@
         <v>0.44166666666666665</v>
       </c>
     </row>
-    <row r="88" spans="1:57" ht="176.1">
+    <row r="88" spans="1:57" ht="176" x14ac:dyDescent="0.2">
       <c r="A88" s="6">
         <v>7507977</v>
       </c>
@@ -11952,7 +13412,7 @@
         <v>0.53333333333333333</v>
       </c>
     </row>
-    <row r="89" spans="1:57" ht="144">
+    <row r="89" spans="1:57" ht="144" x14ac:dyDescent="0.2">
       <c r="A89" s="6">
         <v>8305938</v>
       </c>
@@ -12032,7 +13492,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="90" spans="1:57" ht="144">
+    <row r="90" spans="1:57" ht="144" x14ac:dyDescent="0.2">
       <c r="A90" s="6">
         <v>7100474</v>
       </c>
@@ -12109,7 +13569,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="91" spans="1:57" ht="192">
+    <row r="91" spans="1:57" ht="192" x14ac:dyDescent="0.2">
       <c r="A91" s="6">
         <v>8453107</v>
       </c>
@@ -12192,7 +13652,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="92" spans="1:57" ht="255.95">
+    <row r="92" spans="1:57" ht="256" x14ac:dyDescent="0.2">
       <c r="A92" s="6">
         <v>9464569</v>
       </c>
@@ -12275,7 +13735,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="93" spans="1:57" ht="224.1">
+    <row r="93" spans="1:57" ht="224" x14ac:dyDescent="0.2">
       <c r="A93" s="6">
         <v>9616824</v>
       </c>
@@ -12355,7 +13815,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="94" spans="1:57" ht="159.94999999999999">
+    <row r="94" spans="1:57" ht="160" x14ac:dyDescent="0.2">
       <c r="A94" s="6">
         <v>9155903</v>
       </c>
@@ -12435,7 +13895,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="95" spans="1:57" ht="224.1">
+    <row r="95" spans="1:57" ht="224" x14ac:dyDescent="0.2">
       <c r="A95" s="6">
         <v>10493937</v>
       </c>
@@ -12515,7 +13975,7 @@
         <v>0.3666666666666667</v>
       </c>
     </row>
-    <row r="96" spans="1:57" ht="111.95">
+    <row r="96" spans="1:57" ht="112" x14ac:dyDescent="0.2">
       <c r="A96" s="6">
         <v>7828927</v>
       </c>
@@ -12595,7 +14055,7 @@
         <v>0.3666666666666667</v>
       </c>
     </row>
-    <row r="97" spans="1:61" ht="176.1">
+    <row r="97" spans="1:61" ht="176" x14ac:dyDescent="0.2">
       <c r="A97" s="6">
         <v>10660677</v>
       </c>
@@ -12675,7 +14135,7 @@
         <v>0.39166666666666666</v>
       </c>
     </row>
-    <row r="98" spans="1:61" ht="176.1">
+    <row r="98" spans="1:61" ht="176" x14ac:dyDescent="0.2">
       <c r="A98" s="6">
         <v>8754416</v>
       </c>
@@ -12761,7 +14221,7 @@
         <v>0.6166666666666667</v>
       </c>
     </row>
-    <row r="99" spans="1:61" ht="176.1">
+    <row r="99" spans="1:61" ht="176" x14ac:dyDescent="0.2">
       <c r="A99" s="6">
         <v>7582788</v>
       </c>
@@ -12838,7 +14298,7 @@
         <v>0.71666666666666667</v>
       </c>
     </row>
-    <row r="100" spans="1:61" ht="224.1">
+    <row r="100" spans="1:61" ht="224" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
         <v>852</v>
       </c>
@@ -12936,7 +14396,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="101" spans="1:61" ht="176.1">
+    <row r="101" spans="1:61" ht="176" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
         <v>866</v>
       </c>
@@ -13041,7 +14501,7 @@
         <v>0.93333333333333335</v>
       </c>
     </row>
-    <row r="102" spans="1:61" ht="240">
+    <row r="102" spans="1:61" ht="240" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
         <v>879</v>
       </c>
@@ -13127,7 +14587,7 @@
         <v>0.83333333333333326</v>
       </c>
     </row>
-    <row r="103" spans="1:61" ht="192">
+    <row r="103" spans="1:61" ht="192" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
         <v>890</v>
       </c>
@@ -13213,7 +14673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:61" ht="176.1">
+    <row r="104" spans="1:61" ht="176" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
         <v>899</v>
       </c>
@@ -13302,7 +14762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:61" ht="207.95">
+    <row r="105" spans="1:61" ht="208" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
         <v>909</v>
       </c>
@@ -13388,7 +14848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:61" ht="365.1">
+    <row r="106" spans="1:61" ht="365" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
         <v>918</v>
       </c>
@@ -13474,7 +14934,7 @@
         <v>0.83333333333333326</v>
       </c>
     </row>
-    <row r="107" spans="1:61" ht="207.95">
+    <row r="107" spans="1:61" ht="208" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
         <v>929</v>
       </c>
@@ -13560,7 +15020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:61" ht="255.95">
+    <row r="108" spans="1:61" ht="256" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
         <v>938</v>
       </c>
@@ -13652,7 +15112,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="109" spans="1:61" ht="224.1">
+    <row r="109" spans="1:61" ht="224" x14ac:dyDescent="0.2">
       <c r="A109" s="6" t="s">
         <v>951</v>
       </c>
@@ -13738,7 +15198,7 @@
         <v>0.93333333333333335</v>
       </c>
     </row>
-    <row r="110" spans="1:61" ht="209.1" thickBot="1">
+    <row r="110" spans="1:61" ht="209" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
         <v>960</v>
       </c>
@@ -13824,7 +15284,7 @@
         <v>0.93333333333333335</v>
       </c>
     </row>
-    <row r="111" spans="1:61" ht="96.95" thickBot="1">
+    <row r="111" spans="1:61" ht="97" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C111" s="7" t="s">
         <v>969</v>
       </c>
@@ -13883,7 +15343,7 @@
         <v>0.53333333333333333</v>
       </c>
     </row>
-    <row r="112" spans="1:61" ht="177" thickBot="1">
+    <row r="112" spans="1:61" ht="177" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C112" s="7" t="s">
         <v>973</v>
       </c>
@@ -13958,7 +15418,7 @@
         <v>0.90833333333333321</v>
       </c>
     </row>
-    <row r="113" spans="3:57" ht="192.95" thickBot="1">
+    <row r="113" spans="3:57" ht="193" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C113" s="7" t="s">
         <v>977</v>
       </c>
@@ -14017,7 +15477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="3:57" ht="128.1">
+    <row r="114" spans="3:57" ht="128" x14ac:dyDescent="0.2">
       <c r="C114" s="7" t="s">
         <v>981</v>
       </c>
@@ -14086,7 +15546,7 @@
         <v>0.54625000000000001</v>
       </c>
     </row>
-    <row r="115" spans="3:57" ht="128.1">
+    <row r="115" spans="3:57" ht="128" x14ac:dyDescent="0.2">
       <c r="C115" s="7" t="s">
         <v>985</v>
       </c>
@@ -14145,7 +15605,7 @@
         <v>0.73333333333333339</v>
       </c>
     </row>
-    <row r="116" spans="3:57" ht="144">
+    <row r="116" spans="3:57" ht="144" x14ac:dyDescent="0.2">
       <c r="C116" s="7" t="s">
         <v>989</v>
       </c>
@@ -14204,7 +15664,7 @@
         <v>0.71666666666666667</v>
       </c>
     </row>
-    <row r="117" spans="3:57" ht="96">
+    <row r="117" spans="3:57" ht="96" x14ac:dyDescent="0.2">
       <c r="C117" s="7" t="s">
         <v>993</v>
       </c>
@@ -14277,7 +15737,7 @@
         <v>0.52499999999999991</v>
       </c>
     </row>
-    <row r="118" spans="3:57" ht="65.099999999999994" thickBot="1">
+    <row r="118" spans="3:57" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C118" s="7" t="s">
         <v>997</v>
       </c>
@@ -14348,7 +15808,7 @@
         <v>0.745</v>
       </c>
     </row>
-    <row r="119" spans="3:57" ht="129" thickBot="1">
+    <row r="119" spans="3:57" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C119" s="7" t="s">
         <v>1001</v>
       </c>
@@ -14423,7 +15883,7 @@
         <v>0.96666666666666656</v>
       </c>
     </row>
-    <row r="120" spans="3:57" ht="111.95">
+    <row r="120" spans="3:57" ht="112" x14ac:dyDescent="0.2">
       <c r="C120" s="7" t="s">
         <v>1004</v>
       </c>
@@ -14498,7 +15958,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="121" spans="3:57" ht="144">
+    <row r="121" spans="3:57" ht="144" x14ac:dyDescent="0.2">
       <c r="C121" s="7" t="s">
         <v>1008</v>
       </c>
@@ -14561,7 +16021,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="122" spans="3:57" ht="303.95">
+    <row r="122" spans="3:57" ht="304" x14ac:dyDescent="0.2">
       <c r="C122" s="7" t="s">
         <v>1012</v>
       </c>
@@ -14620,7 +16080,7 @@
         <v>0.8833333333333333</v>
       </c>
     </row>
-    <row r="123" spans="3:57" ht="111.95">
+    <row r="123" spans="3:57" ht="112" x14ac:dyDescent="0.2">
       <c r="C123" s="7" t="s">
         <v>1016</v>
       </c>
@@ -14679,7 +16139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="3:57" ht="128.1">
+    <row r="124" spans="3:57" ht="128" x14ac:dyDescent="0.2">
       <c r="C124" s="7" t="s">
         <v>1018</v>
       </c>
@@ -14738,7 +16198,7 @@
         <v>0.83333333333333326</v>
       </c>
     </row>
-    <row r="125" spans="3:57" ht="207.95">
+    <row r="125" spans="3:57" ht="208" x14ac:dyDescent="0.2">
       <c r="C125" s="7" t="s">
         <v>1022</v>
       </c>
@@ -14813,7 +16273,7 @@
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="126" spans="3:57" ht="144">
+    <row r="126" spans="3:57" ht="144" x14ac:dyDescent="0.2">
       <c r="C126" s="7" t="s">
         <v>1026</v>
       </c>
@@ -14872,7 +16332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="3:57" ht="159.94999999999999">
+    <row r="127" spans="3:57" ht="160" x14ac:dyDescent="0.2">
       <c r="C127" s="7" t="s">
         <v>1030</v>
       </c>
@@ -14947,7 +16407,7 @@
         <v>0.90833333333333321</v>
       </c>
     </row>
-    <row r="128" spans="3:57" ht="128.1">
+    <row r="128" spans="3:57" ht="128" x14ac:dyDescent="0.2">
       <c r="C128" s="7" t="s">
         <v>1034</v>
       </c>
@@ -15006,7 +16466,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="129" spans="3:61" ht="111.95">
+    <row r="129" spans="3:61" ht="112" x14ac:dyDescent="0.2">
       <c r="C129" s="7" t="s">
         <v>1038</v>
       </c>
@@ -15065,7 +16525,7 @@
         <v>0.6333333333333333</v>
       </c>
     </row>
-    <row r="130" spans="3:61" ht="176.1">
+    <row r="130" spans="3:61" ht="176" x14ac:dyDescent="0.2">
       <c r="C130" s="7" t="s">
         <v>1042</v>
       </c>
@@ -15143,7 +16603,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="131" spans="3:61" ht="144">
+    <row r="131" spans="3:61" ht="144" x14ac:dyDescent="0.2">
       <c r="C131" s="7" t="s">
         <v>1047</v>
       </c>
@@ -15202,7 +16662,7 @@
         <v>0.94166666666666665</v>
       </c>
     </row>
-    <row r="132" spans="3:61" ht="159.94999999999999">
+    <row r="132" spans="3:61" ht="160" x14ac:dyDescent="0.2">
       <c r="C132" s="7" t="s">
         <v>1051</v>
       </c>
@@ -15261,7 +16721,7 @@
         <v>0.60833333333333328</v>
       </c>
     </row>
-    <row r="133" spans="3:61" ht="144">
+    <row r="133" spans="3:61" ht="144" x14ac:dyDescent="0.2">
       <c r="C133" s="7" t="s">
         <v>1055</v>
       </c>
@@ -15320,7 +16780,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="134" spans="3:61" ht="176.1">
+    <row r="134" spans="3:61" ht="176" x14ac:dyDescent="0.2">
       <c r="C134" s="7" t="s">
         <v>1059</v>
       </c>
@@ -15379,7 +16839,7 @@
         <v>0.83333333333333326</v>
       </c>
     </row>
-    <row r="135" spans="3:61" ht="240">
+    <row r="135" spans="3:61" ht="240" x14ac:dyDescent="0.2">
       <c r="C135" s="7" t="s">
         <v>1063</v>
       </c>
@@ -15438,7 +16898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="3:61" ht="144">
+    <row r="136" spans="3:61" ht="144" x14ac:dyDescent="0.2">
       <c r="C136" s="7" t="s">
         <v>1067</v>
       </c>
@@ -15497,7 +16957,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="137" spans="3:61" ht="96">
+    <row r="137" spans="3:61" ht="96" x14ac:dyDescent="0.2">
       <c r="C137" s="7" t="s">
         <v>1071</v>
       </c>
@@ -15556,7 +17016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="3:61" ht="176.1">
+    <row r="138" spans="3:61" ht="176" x14ac:dyDescent="0.2">
       <c r="C138" s="7" t="s">
         <v>1075</v>
       </c>
@@ -15615,7 +17075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="3:61" ht="176.1">
+    <row r="139" spans="3:61" ht="176" x14ac:dyDescent="0.2">
       <c r="C139" s="7" t="s">
         <v>1079</v>
       </c>
@@ -15677,7 +17137,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="140" spans="3:61" ht="255.95">
+    <row r="140" spans="3:61" ht="256" x14ac:dyDescent="0.2">
       <c r="C140" s="7" t="s">
         <v>1084</v>
       </c>
@@ -15736,7 +17196,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="141" spans="3:61" ht="320.10000000000002">
+    <row r="141" spans="3:61" ht="320" x14ac:dyDescent="0.2">
       <c r="C141" s="7" t="s">
         <v>1087</v>
       </c>
@@ -15795,7 +17255,7 @@
         <v>0.83333333333333326</v>
       </c>
     </row>
-    <row r="142" spans="3:61" ht="128.1">
+    <row r="142" spans="3:61" ht="128" x14ac:dyDescent="0.2">
       <c r="C142" s="7" t="s">
         <v>1091</v>
       </c>
@@ -15854,7 +17314,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="143" spans="3:61" ht="111.95">
+    <row r="143" spans="3:61" ht="112" x14ac:dyDescent="0.2">
       <c r="C143" s="7" t="s">
         <v>1095</v>
       </c>
@@ -15913,7 +17373,7 @@
         <v>0.96666666666666667</v>
       </c>
     </row>
-    <row r="144" spans="3:61" ht="159.94999999999999">
+    <row r="144" spans="3:61" ht="160" x14ac:dyDescent="0.2">
       <c r="C144" s="7" t="s">
         <v>1099</v>
       </c>
@@ -15972,7 +17432,7 @@
         <v>0.71666666666666667</v>
       </c>
     </row>
-    <row r="145" spans="3:57" ht="144">
+    <row r="145" spans="3:57" ht="144" x14ac:dyDescent="0.2">
       <c r="C145" s="7" t="s">
         <v>1103</v>
       </c>
@@ -16031,7 +17491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="3:57" ht="192">
+    <row r="146" spans="3:57" ht="192" x14ac:dyDescent="0.2">
       <c r="C146" s="7" t="s">
         <v>1107</v>
       </c>
@@ -16090,7 +17550,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="147" spans="3:57" ht="128.1">
+    <row r="147" spans="3:57" ht="128" x14ac:dyDescent="0.2">
       <c r="C147" s="7" t="s">
         <v>1111</v>
       </c>
@@ -16149,7 +17609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="3:57" ht="144">
+    <row r="148" spans="3:57" ht="144" x14ac:dyDescent="0.2">
       <c r="C148" s="7" t="s">
         <v>1115</v>
       </c>
@@ -16208,7 +17668,7 @@
         <v>0.7583333333333333</v>
       </c>
     </row>
-    <row r="149" spans="3:57" ht="176.1">
+    <row r="149" spans="3:57" ht="176" x14ac:dyDescent="0.2">
       <c r="C149" s="7" t="s">
         <v>1119</v>
       </c>
@@ -16267,7 +17727,7 @@
         <v>0.96666666666666667</v>
       </c>
     </row>
-    <row r="150" spans="3:57" ht="144">
+    <row r="150" spans="3:57" ht="144" x14ac:dyDescent="0.2">
       <c r="C150" s="7" t="s">
         <v>1123</v>
       </c>
@@ -16326,7 +17786,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="151" spans="3:57" ht="224.1">
+    <row r="151" spans="3:57" ht="224" x14ac:dyDescent="0.2">
       <c r="C151" s="7" t="s">
         <v>1127</v>
       </c>
@@ -16385,7 +17845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="3:57" ht="176.1">
+    <row r="152" spans="3:57" ht="176" x14ac:dyDescent="0.2">
       <c r="C152" s="7" t="s">
         <v>1131</v>
       </c>
@@ -16444,7 +17904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="3:57" ht="96">
+    <row r="153" spans="3:57" ht="96" x14ac:dyDescent="0.2">
       <c r="C153" s="7" t="s">
         <v>1135</v>
       </c>
@@ -16503,7 +17963,7 @@
         <v>0.83333333333333326</v>
       </c>
     </row>
-    <row r="154" spans="3:57" ht="128.1">
+    <row r="154" spans="3:57" ht="128" x14ac:dyDescent="0.2">
       <c r="C154" s="7" t="s">
         <v>1139</v>
       </c>
@@ -16562,7 +18022,7 @@
         <v>0.53333333333333333</v>
       </c>
     </row>
-    <row r="155" spans="3:57" ht="159.94999999999999">
+    <row r="155" spans="3:57" ht="160" x14ac:dyDescent="0.2">
       <c r="C155" s="7" t="s">
         <v>1143</v>
       </c>
@@ -16621,7 +18081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="3:57" ht="207.95">
+    <row r="156" spans="3:57" ht="208" x14ac:dyDescent="0.2">
       <c r="C156" s="7" t="s">
         <v>1147</v>
       </c>
@@ -16680,7 +18140,7 @@
         <v>0.93333333333333335</v>
       </c>
     </row>
-    <row r="157" spans="3:57" ht="96">
+    <row r="157" spans="3:57" ht="96" x14ac:dyDescent="0.2">
       <c r="C157" s="7" t="s">
         <v>1151</v>
       </c>
@@ -16739,7 +18199,7 @@
         <v>0.71666666666666667</v>
       </c>
     </row>
-    <row r="158" spans="3:57" ht="159.94999999999999">
+    <row r="158" spans="3:57" ht="160" x14ac:dyDescent="0.2">
       <c r="C158" s="7" t="s">
         <v>1155</v>
       </c>
@@ -16798,7 +18258,7 @@
         <v>0.53333333333333333</v>
       </c>
     </row>
-    <row r="159" spans="3:57" ht="128.1">
+    <row r="159" spans="3:57" ht="128" x14ac:dyDescent="0.2">
       <c r="C159" s="7" t="s">
         <v>1159</v>
       </c>
@@ -16857,7 +18317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="3:57" ht="144">
+    <row r="160" spans="3:57" ht="144" x14ac:dyDescent="0.2">
       <c r="C160" s="7" t="s">
         <v>1163</v>
       </c>
@@ -16916,7 +18376,7 @@
         <v>0.96666666666666667</v>
       </c>
     </row>
-    <row r="161" spans="3:57" ht="176.1">
+    <row r="161" spans="3:57" ht="176" x14ac:dyDescent="0.2">
       <c r="C161" s="7" t="s">
         <v>1166</v>
       </c>
@@ -16975,7 +18435,7 @@
         <v>0.83333333333333326</v>
       </c>
     </row>
-    <row r="162" spans="3:57" ht="176.1">
+    <row r="162" spans="3:57" ht="176" x14ac:dyDescent="0.2">
       <c r="C162" s="7" t="s">
         <v>1170</v>
       </c>
@@ -17034,7 +18494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="3:57" ht="159.94999999999999">
+    <row r="163" spans="3:57" ht="160" x14ac:dyDescent="0.2">
       <c r="C163" s="7" t="s">
         <v>1173</v>
       </c>
@@ -17093,7 +18553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="3:57" ht="176.1">
+    <row r="164" spans="3:57" ht="176" x14ac:dyDescent="0.2">
       <c r="C164" s="7" t="s">
         <v>1176</v>
       </c>
@@ -17152,7 +18612,7 @@
         <v>0.51666666666666661</v>
       </c>
     </row>
-    <row r="165" spans="3:57" ht="111.95">
+    <row r="165" spans="3:57" ht="112" x14ac:dyDescent="0.2">
       <c r="C165" s="7" t="s">
         <v>1180</v>
       </c>
@@ -17167,9 +18627,6 @@
       </c>
       <c r="J165" s="7" t="s">
         <v>1183</v>
-      </c>
-      <c r="AN165" s="13" t="s">
-        <v>78</v>
       </c>
       <c r="AO165" s="13">
         <v>0.8</v>
@@ -17211,7 +18668,7 @@
         <v>0.73333333333333339</v>
       </c>
     </row>
-    <row r="166" spans="3:57" ht="128.1">
+    <row r="166" spans="3:57" ht="128" x14ac:dyDescent="0.2">
       <c r="C166" s="7" t="s">
         <v>1184</v>
       </c>
@@ -17270,7 +18727,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="167" spans="3:57" ht="176.1">
+    <row r="167" spans="3:57" ht="176" x14ac:dyDescent="0.2">
       <c r="C167" s="7" t="s">
         <v>1188</v>
       </c>
@@ -17329,7 +18786,7 @@
         <v>0.83333333333333326</v>
       </c>
     </row>
-    <row r="168" spans="3:57" ht="192">
+    <row r="168" spans="3:57" ht="192" x14ac:dyDescent="0.2">
       <c r="C168" s="7" t="s">
         <v>1191</v>
       </c>
@@ -17388,7 +18845,7 @@
         <v>0.56666666666666665</v>
       </c>
     </row>
-    <row r="169" spans="3:57" ht="111.95">
+    <row r="169" spans="3:57" ht="112" x14ac:dyDescent="0.2">
       <c r="C169" s="7" t="s">
         <v>1195</v>
       </c>
@@ -17447,7 +18904,7 @@
         <v>0.56666666666666665</v>
       </c>
     </row>
-    <row r="170" spans="3:57" ht="144">
+    <row r="170" spans="3:57" ht="144" x14ac:dyDescent="0.2">
       <c r="C170" s="7" t="s">
         <v>1199</v>
       </c>
@@ -17506,7 +18963,7 @@
         <v>0.76666666666666661</v>
       </c>
     </row>
-    <row r="171" spans="3:57" ht="159.94999999999999">
+    <row r="171" spans="3:57" ht="160" x14ac:dyDescent="0.2">
       <c r="C171" s="7" t="s">
         <v>1203</v>
       </c>
@@ -17579,7 +19036,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="172" spans="3:57" ht="159.94999999999999">
+    <row r="172" spans="3:57" ht="160" x14ac:dyDescent="0.2">
       <c r="C172" s="7" t="s">
         <v>1206</v>
       </c>
@@ -17638,7 +19095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="3:57" ht="159.94999999999999">
+    <row r="173" spans="3:57" ht="160" x14ac:dyDescent="0.2">
       <c r="C173" s="7" t="s">
         <v>1210</v>
       </c>
@@ -17697,7 +19154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="3:57" ht="159.94999999999999">
+    <row r="174" spans="3:57" ht="160" x14ac:dyDescent="0.2">
       <c r="C174" s="7" t="s">
         <v>1213</v>
       </c>
@@ -17756,7 +19213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="3:57" ht="144">
+    <row r="175" spans="3:57" ht="144" x14ac:dyDescent="0.2">
       <c r="C175" s="7" t="s">
         <v>1217</v>
       </c>
@@ -17831,7 +19288,7 @@
         <v>0.77083333333333337</v>
       </c>
     </row>
-    <row r="176" spans="3:57" ht="144">
+    <row r="176" spans="3:57" ht="144" x14ac:dyDescent="0.2">
       <c r="C176" s="7" t="s">
         <v>1221</v>
       </c>
@@ -17890,7 +19347,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="177" spans="3:57" ht="159.94999999999999">
+    <row r="177" spans="3:57" ht="160" x14ac:dyDescent="0.2">
       <c r="C177" s="7" t="s">
         <v>1225</v>
       </c>
@@ -17949,7 +19406,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="178" spans="3:57" ht="111.95">
+    <row r="178" spans="3:57" ht="112" x14ac:dyDescent="0.2">
       <c r="C178" s="7" t="s">
         <v>1229</v>
       </c>
@@ -18008,7 +19465,7 @@
         <v>0.51666666666666661</v>
       </c>
     </row>
-    <row r="179" spans="3:57" ht="96">
+    <row r="179" spans="3:57" ht="96" x14ac:dyDescent="0.2">
       <c r="C179" s="7" t="s">
         <v>1233</v>
       </c>
@@ -18067,7 +19524,7 @@
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="180" spans="3:57" ht="128.1">
+    <row r="180" spans="3:57" ht="128" x14ac:dyDescent="0.2">
       <c r="C180" s="7" t="s">
         <v>1237</v>
       </c>
@@ -18126,7 +19583,7 @@
         <v>0.58333333333333326</v>
       </c>
     </row>
-    <row r="181" spans="3:57" ht="192">
+    <row r="181" spans="3:57" ht="192" x14ac:dyDescent="0.2">
       <c r="C181" s="7" t="s">
         <v>1241</v>
       </c>
@@ -18201,7 +19658,7 @@
         <v>0.72083333333333333</v>
       </c>
     </row>
-    <row r="182" spans="3:57" ht="128.1">
+    <row r="182" spans="3:57" ht="128" x14ac:dyDescent="0.2">
       <c r="C182" s="7" t="s">
         <v>1245</v>
       </c>
@@ -18272,7 +19729,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="183" spans="3:57" ht="96">
+    <row r="183" spans="3:57" ht="96" x14ac:dyDescent="0.2">
       <c r="C183" s="7" t="s">
         <v>1249</v>
       </c>
@@ -18345,7 +19802,7 @@
         <v>0.43499999999999994</v>
       </c>
     </row>
-    <row r="184" spans="3:57" ht="159.94999999999999">
+    <row r="184" spans="3:57" ht="160" x14ac:dyDescent="0.2">
       <c r="C184" s="7" t="s">
         <v>1254</v>
       </c>
@@ -18404,7 +19861,7 @@
         <v>0.76666666666666661</v>
       </c>
     </row>
-    <row r="185" spans="3:57" ht="207.95">
+    <row r="185" spans="3:57" ht="208" x14ac:dyDescent="0.2">
       <c r="C185" s="7" t="s">
         <v>1258</v>
       </c>
@@ -18463,7 +19920,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="186" spans="3:57" ht="192">
+    <row r="186" spans="3:57" ht="192" x14ac:dyDescent="0.2">
       <c r="C186" s="7" t="s">
         <v>1262</v>
       </c>
@@ -18522,7 +19979,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="187" spans="3:57" ht="96">
+    <row r="187" spans="3:57" ht="96" x14ac:dyDescent="0.2">
       <c r="C187" s="7" t="s">
         <v>1266</v>
       </c>
@@ -18581,7 +20038,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="188" spans="3:57" ht="80.099999999999994">
+    <row r="188" spans="3:57" ht="80" x14ac:dyDescent="0.2">
       <c r="C188" s="7" t="s">
         <v>1270</v>
       </c>
@@ -18640,7 +20097,7 @@
         <v>0.81666666666666665</v>
       </c>
     </row>
-    <row r="189" spans="3:57" ht="176.1">
+    <row r="189" spans="3:57" ht="176" x14ac:dyDescent="0.2">
       <c r="C189" s="7" t="s">
         <v>1274</v>
       </c>
@@ -18699,7 +20156,7 @@
         <v>0.71666666666666667</v>
       </c>
     </row>
-    <row r="190" spans="3:57" ht="159.94999999999999">
+    <row r="190" spans="3:57" ht="160" x14ac:dyDescent="0.2">
       <c r="C190" s="7" t="s">
         <v>1278</v>
       </c>
@@ -18758,7 +20215,7 @@
         <v>0.93333333333333335</v>
       </c>
     </row>
-    <row r="191" spans="3:57" ht="144">
+    <row r="191" spans="3:57" ht="144" x14ac:dyDescent="0.2">
       <c r="C191" s="7" t="s">
         <v>1282</v>
       </c>
@@ -18817,7 +20274,7 @@
         <v>0.68333333333333335</v>
       </c>
     </row>
-    <row r="192" spans="3:57" ht="128.1">
+    <row r="192" spans="3:57" ht="128" x14ac:dyDescent="0.2">
       <c r="C192" s="7" t="s">
         <v>1286</v>
       </c>
@@ -18876,7 +20333,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="193" spans="3:57" ht="192">
+    <row r="193" spans="3:57" ht="192" x14ac:dyDescent="0.2">
       <c r="C193" s="7" t="s">
         <v>1290</v>
       </c>
@@ -18935,7 +20392,7 @@
         <v>0.81666666666666665</v>
       </c>
     </row>
-    <row r="194" spans="3:57" ht="144">
+    <row r="194" spans="3:57" ht="144" x14ac:dyDescent="0.2">
       <c r="C194" s="7" t="s">
         <v>1294</v>
       </c>
@@ -18994,7 +20451,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="195" spans="3:57" ht="159.94999999999999">
+    <row r="195" spans="3:57" ht="160" x14ac:dyDescent="0.2">
       <c r="C195" s="7" t="s">
         <v>1298</v>
       </c>
@@ -19069,7 +20526,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="196" spans="3:57" ht="176.1">
+    <row r="196" spans="3:57" ht="176" x14ac:dyDescent="0.2">
       <c r="C196" s="7" t="s">
         <v>1302</v>
       </c>
@@ -19128,7 +20585,7 @@
         <v>0.8833333333333333</v>
       </c>
     </row>
-    <row r="197" spans="3:57" ht="159.94999999999999">
+    <row r="197" spans="3:57" ht="160" x14ac:dyDescent="0.2">
       <c r="C197" s="7" t="s">
         <v>1305</v>
       </c>
@@ -19187,7 +20644,7 @@
         <v>0.84166666666666667</v>
       </c>
     </row>
-    <row r="198" spans="3:57" ht="159.94999999999999">
+    <row r="198" spans="3:57" ht="160" x14ac:dyDescent="0.2">
       <c r="C198" s="7" t="s">
         <v>1309</v>
       </c>
@@ -19246,7 +20703,7 @@
         <v>0.76666666666666672</v>
       </c>
     </row>
-    <row r="199" spans="3:57" ht="111.95">
+    <row r="199" spans="3:57" ht="112" x14ac:dyDescent="0.2">
       <c r="C199" s="7" t="s">
         <v>1313</v>
       </c>
@@ -19316,7 +20773,7 @@
         <v>0.42416666666666669</v>
       </c>
     </row>
-    <row r="200" spans="3:57" ht="192">
+    <row r="200" spans="3:57" ht="192" x14ac:dyDescent="0.2">
       <c r="C200" s="7" t="s">
         <v>1316</v>
       </c>
@@ -19375,7 +20832,7 @@
         <v>0.7416666666666667</v>
       </c>
     </row>
-    <row r="201" spans="3:57" ht="176.1">
+    <row r="201" spans="3:57" ht="176" x14ac:dyDescent="0.2">
       <c r="C201" s="7" t="s">
         <v>1320</v>
       </c>
@@ -19434,7 +20891,7 @@
         <v>0.71666666666666667</v>
       </c>
     </row>
-    <row r="202" spans="3:57" ht="288">
+    <row r="202" spans="3:57" ht="288" x14ac:dyDescent="0.2">
       <c r="C202" s="7" t="s">
         <v>1323</v>
       </c>
@@ -19493,7 +20950,7 @@
         <v>0.58333333333333326</v>
       </c>
     </row>
-    <row r="203" spans="3:57" ht="128.1">
+    <row r="203" spans="3:57" ht="128" x14ac:dyDescent="0.2">
       <c r="C203" s="7" t="s">
         <v>1327</v>
       </c>
@@ -19578,7 +21035,8 @@
     <hyperlink ref="S110" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId22"/>
+  <drawing r:id="rId22"/>
+  <legacyDrawing r:id="rId23"/>
 </worksheet>
 </file>
 
@@ -19798,13 +21256,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75C2E995-E4B5-43AB-976A-D7C66C193ADA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75C2E995-E4B5-43AB-976A-D7C66C193ADA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ab92c565-5003-4ac3-93a3-a3ce8796a3c0"/>
+    <ds:schemaRef ds:uri="aa1b21cb-23df-461b-8b8e-4aaeac2f3f50"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{943FC6A1-4453-4C1A-9E7F-BF39CEFF06B8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{943FC6A1-4453-4C1A-9E7F-BF39CEFF06B8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E930122-8DA5-429F-A725-BB94052D8ABA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E930122-8DA5-429F-A725-BB94052D8ABA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ab92c565-5003-4ac3-93a3-a3ce8796a3c0"/>
+    <ds:schemaRef ds:uri="aa1b21cb-23df-461b-8b8e-4aaeac2f3f50"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>